<commit_message>
Allowing for variable MCQ-s options.
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="29">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">info</t>
   </si>
   <si>
-    <t xml:space="preserve">Q</t>
+    <t xml:space="preserve">question</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t xml:space="preserve">Option D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The answer</t>
   </si>
 </sst>
 </file>
@@ -235,30 +232,30 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.34"/>
@@ -270,7 +267,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.33"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="10" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="3" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,7 +331,7 @@
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="60.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -368,7 +365,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -391,7 +388,7 @@
         <v>28</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -402,7 +399,7 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -425,7 +422,7 @@
         <v>28</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -436,7 +433,7 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -459,7 +456,7 @@
         <v>28</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -470,7 +467,7 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -493,7 +490,7 @@
         <v>28</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -504,7 +501,7 @@
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -527,7 +524,7 @@
         <v>28</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -538,7 +535,7 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -561,7 +558,7 @@
         <v>28</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -572,7 +569,7 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -595,7 +592,7 @@
         <v>28</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -606,7 +603,7 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -629,7 +626,7 @@
         <v>28</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -640,7 +637,7 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -663,7 +660,7 @@
         <v>28</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -674,7 +671,7 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -697,7 +694,7 @@
         <v>28</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -709,7 +706,7 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -732,7 +729,7 @@
         <v>28</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -743,7 +740,7 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -766,10 +763,10 @@
         <v>28</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -792,10 +789,10 @@
         <v>28</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="21.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -818,7 +815,7 @@
         <v>28</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>